<commit_message>
Relational Model hopefully works on
</commit_message>
<xml_diff>
--- a/fully dressd.xlsx
+++ b/fully dressd.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -46,9 +46,6 @@
     <t>Alternative flows</t>
   </si>
   <si>
-    <t>Process ordering</t>
-  </si>
-  <si>
     <t>Customer, Employee</t>
   </si>
   <si>
@@ -82,7 +79,10 @@
     <t xml:space="preserve">4a. Item is not in stock </t>
   </si>
   <si>
-    <t xml:space="preserve">1.Costumer makes a call and makes an order and specifies information (name,size,type) </t>
+    <t xml:space="preserve">1.Customer makes a call and makes an order and specifies information (name,size,type) </t>
+  </si>
+  <si>
+    <t>makeSale</t>
   </si>
 </sst>
 </file>
@@ -210,6 +210,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -222,12 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -270,21 +282,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -292,14 +292,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -337,9 +340,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,7 +377,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,7 +412,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +589,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G9"/>
+      <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,143 +606,138 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="10"/>
+      <c r="G1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="12"/>
+      <c r="G2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="12"/>
+      <c r="G3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="13"/>
+      <c r="G4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="6:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="19"/>
+      <c r="G8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="19"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="19"/>
+      <c r="G10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="6:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="15"/>
-      <c r="G8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F9" s="15"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="15"/>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="24" t="s">
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="19"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="19"/>
+      <c r="G12" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F11" s="15"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="15"/>
-      <c r="G12" s="23" t="s">
+      <c r="H12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="25" t="s">
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="19"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="26"/>
+      <c r="G14" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="15"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="22"/>
-      <c r="G14" s="19" t="s">
+      <c r="H14" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="20" t="s">
+    </row>
+    <row r="15" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="26"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="22"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="4"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
@@ -756,6 +754,11 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>